<commit_message>
avance sprint 6 encuestas e informes
</commit_message>
<xml_diff>
--- a/Informe_Turnos_Finalizados_Por_Lapso.xlsx
+++ b/Informe_Turnos_Finalizados_Por_Lapso.xlsx
@@ -404,7 +404,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Lapso: 2022-10-10 al 2022-11-14</v>
+        <v>Lapso: 2022-10-24 al 2022-11-22</v>
       </c>
     </row>
     <row r="2">
@@ -417,12 +417,18 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Stefania Beatriz Marco</v>
+        <v>Alberto Chinsky</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Alberto Chinsky</v>
+        <v>Stefania Beatriz Marco</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>